<commit_message>
fixes a bug with oil if veg constraint
</commit_message>
<xml_diff>
--- a/Phase1-answer/Question2-part B/Comparison.xlsx
+++ b/Phase1-answer/Question2-part B/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase1-answer\Question2-part B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80BBB760-BC52-4740-A8A0-EC215D1665FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF83D5F-9D7B-44F4-A0CC-E62E12BF5A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0396B2F8-717D-4DFE-86B2-E6C861481D46}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>revenue</t>
   </si>
@@ -52,6 +52,9 @@
   <si>
     <t>Part A</t>
   </si>
+  <si>
+    <t>Percent Changed</t>
+  </si>
 </sst>
 </file>
 
@@ -60,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +81,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,10 +117,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -118,9 +129,11 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,7 +369,7 @@
                   <c:v>405000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>405000</c:v>
+                  <c:v>398250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -510,7 +523,7 @@
                   <c:v>246493.14236111112</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>251866</c:v>
+                  <c:v>253769</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,7 +674,7 @@
                   <c:v>54119.531250000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56319</c:v>
+                  <c:v>49944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -808,7 +821,7 @@
                   <c:v>104387.32638888888</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96815</c:v>
+                  <c:v>94537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1581,15 +1594,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1914,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8742C1C-484F-4280-B8E0-AD7E2DD3F143}">
-  <dimension ref="C5:E9"/>
+  <dimension ref="C5:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1925,17 +1938,21 @@
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1943,10 +1960,14 @@
         <v>405000</v>
       </c>
       <c r="E6" s="2">
-        <v>405000</v>
+        <v>398250</v>
+      </c>
+      <c r="F6" s="3">
+        <f>(E6-D6)/D6</f>
+        <v>-1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="7" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1954,10 +1975,14 @@
         <v>246493.14236111112</v>
       </c>
       <c r="E7" s="2">
-        <v>251866</v>
+        <v>253769</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" ref="F7:F9" si="0">(E7-D7)/D7</f>
+        <v>2.9517485026945633E-2</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1965,10 +1990,14 @@
         <v>54119.531250000007</v>
       </c>
       <c r="E8" s="2">
-        <v>56319</v>
+        <v>49944</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>-7.7153869472954953E-2</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1976,7 +2005,11 @@
         <v>104387.32638888888</v>
       </c>
       <c r="E9" s="2">
-        <v>96815</v>
+        <v>94537</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.436324053546559E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>